<commit_message>
update lecture 1 and func summ
</commit_message>
<xml_diff>
--- a/Function Summary/Function Summary.xlsx
+++ b/Function Summary/Function Summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirksmith/Documents/Michigan/Chandrasekaran Lab/AI in BME/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirksmith/Documents/Michigan/Chandrasekaran Lab/AI in BME/bme499/Function Summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFD44A6-7A49-374D-9281-C20604B62FC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EF384F-7093-F64F-AB6A-747BA3D1DF96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="13220" windowHeight="15760" xr2:uid="{492C2B8E-C383-D649-9C6E-7282F1980CC8}"/>
+    <workbookView xWindow="1800" yWindow="460" windowWidth="13220" windowHeight="15760" xr2:uid="{492C2B8E-C383-D649-9C6E-7282F1980CC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -570,10 +570,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BEC0F1-F6A1-7645-97C1-52C8B30E59A9}">
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -901,18 +901,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
@@ -1155,10 +1155,10 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
@@ -1297,10 +1297,10 @@
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="1"/>
+      <c r="B53" s="2"/>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
@@ -1423,10 +1423,10 @@
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B70" s="1"/>
+      <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
@@ -1524,5 +1524,6 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>